<commit_message>
Generate all flattend report
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -460,63 +460,231 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>INC001</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>Accident</v>
+        <v/>
       </c>
       <c r="C2" t="str">
-        <v>PIE</v>
+        <v/>
       </c>
       <c r="D2" t="str">
-        <v>towards Tuas</v>
+        <v/>
       </c>
       <c r="E2" t="str">
-        <v>before Eunos Exit</v>
+        <v/>
       </c>
       <c r="F2" t="str">
-        <v>2025-05-17T07:35:00+08:00</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>Ongoing</v>
+        <v/>
       </c>
       <c r="H2" t="str">
-        <v>Car, Motorcycle</v>
+        <v/>
       </c>
       <c r="I2" t="str">
-        <v>SBC1234X, FBA5678Z</v>
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>Moderate, High</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
       </c>
       <c r="L2" t="str">
-        <v>Lane 1, Lane 2</v>
+        <v/>
       </c>
       <c r="M2" t="str">
-        <v>Diversion, Congestion Alert</v>
+        <v/>
       </c>
       <c r="N2" t="str">
-        <v>Use Exit 10A to Eunos Link, Avoid Lane 1 and Lane 2 near the exit, Expect delays of up to 25 minutes, Heavy traffic from Kallang Way to Eunos</v>
+        <v/>
       </c>
       <c r="O2" t="str">
-        <v>Traffic Police, SCDF</v>
+        <v/>
       </c>
       <c r="P2" t="str">
-        <v>2025-05-17T07:45:00+08:00, 2025-05-17T07:50:00+08:00</v>
+        <v/>
       </c>
       <c r="Q2" t="str">
-        <v>Sgt. Tan Wei, Cpl. Lim Hui, Lt. Ravi Kumar, Spec. Ong Jia</v>
+        <v/>
       </c>
       <c r="R2" t="str">
-        <v>Team Leader, Traffic Control, Rescue Operations, Paramedic</v>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v/>
+      </c>
+      <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <v/>
+      </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
+        <v/>
+      </c>
+      <c r="O3" t="str">
+        <v/>
+      </c>
+      <c r="P3" t="str">
+        <v/>
+      </c>
+      <c r="Q3" t="str">
+        <v/>
+      </c>
+      <c r="R3" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v/>
+      </c>
+      <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <v/>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <v/>
+      </c>
+      <c r="P4" t="str">
+        <v/>
+      </c>
+      <c r="Q4" t="str">
+        <v/>
+      </c>
+      <c r="R4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+      <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v/>
+      </c>
+      <c r="E5" t="str">
+        <v/>
+      </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v/>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v/>
+      </c>
+      <c r="N5" t="str">
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <v/>
+      </c>
+      <c r="Q5" t="str">
+        <v/>
+      </c>
+      <c r="R5" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:R5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>